<commit_message>
implemented everithing but mail sending and crossing ticket tbd: get mail from sumup mail!
</commit_message>
<xml_diff>
--- a/Alaia Tickets/Alaiavouchers.xlsx
+++ b/Alaia Tickets/Alaiavouchers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/02c612f151501b63/Vereine/ASC CH/Mitgliederverwaltung Programm/Alaia Tickets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="8_{800AA084-8F6B-4FB2-A845-B1F642EBBD10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8A2548F1-8236-43F2-9598-47AFD1241F40}"/>
+  <xr:revisionPtr revIDLastSave="18" documentId="8_{800AA084-8F6B-4FB2-A845-B1F642EBBD10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7C29C0C1-160C-425E-ACBD-31D5E52A14A1}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="24496" windowHeight="15796" xr2:uid="{A1ED1F4A-0D88-4E84-9422-762530081D51}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="116">
   <si>
     <t>Voucher</t>
   </si>
@@ -43,26 +43,362 @@
     <t>Full Name</t>
   </si>
   <si>
-    <t>Order nr</t>
-  </si>
-  <si>
     <t>Date</t>
   </si>
   <si>
-    <t>Email Sent?</t>
-  </si>
-  <si>
-    <t>ASCTEST</t>
+    <t>ASCTEST2</t>
+  </si>
+  <si>
+    <t>ASCTEST1</t>
+  </si>
+  <si>
+    <t>ASCTEST3</t>
+  </si>
+  <si>
+    <t>ASCTEST4</t>
+  </si>
+  <si>
+    <t>ASCTEST5</t>
+  </si>
+  <si>
+    <t>ASCTEST6</t>
+  </si>
+  <si>
+    <t>ASCTEST7</t>
+  </si>
+  <si>
+    <t>ASCTEST8</t>
+  </si>
+  <si>
+    <t>ASCTEST9</t>
+  </si>
+  <si>
+    <t>ASCTEST10</t>
+  </si>
+  <si>
+    <t>ASCTEST11</t>
+  </si>
+  <si>
+    <t>ASCTEST12</t>
+  </si>
+  <si>
+    <t>ASCTEST13</t>
+  </si>
+  <si>
+    <t>ASCTEST14</t>
+  </si>
+  <si>
+    <t>ASCTEST15</t>
+  </si>
+  <si>
+    <t>ASCTEST16</t>
+  </si>
+  <si>
+    <t>ASCTEST17</t>
+  </si>
+  <si>
+    <t>ASCTEST18</t>
+  </si>
+  <si>
+    <t>ASCTEST19</t>
+  </si>
+  <si>
+    <t>ASCTEST20</t>
+  </si>
+  <si>
+    <t>ASCTEST21</t>
+  </si>
+  <si>
+    <t>ASCTEST22</t>
+  </si>
+  <si>
+    <t>ASCTEST23</t>
+  </si>
+  <si>
+    <t>ASCTEST24</t>
+  </si>
+  <si>
+    <t>ASCTEST25</t>
+  </si>
+  <si>
+    <t>ASCTEST26</t>
+  </si>
+  <si>
+    <t>ASCTEST27</t>
+  </si>
+  <si>
+    <t>ASCTEST28</t>
+  </si>
+  <si>
+    <t>ASCTEST29</t>
+  </si>
+  <si>
+    <t>ASCTEST30</t>
+  </si>
+  <si>
+    <t>ASCTEST31</t>
+  </si>
+  <si>
+    <t>ASCTEST32</t>
+  </si>
+  <si>
+    <t>ASCTEST33</t>
+  </si>
+  <si>
+    <t>ASCTEST34</t>
+  </si>
+  <si>
+    <t>ASCTEST35</t>
+  </si>
+  <si>
+    <t>ASCTEST36</t>
+  </si>
+  <si>
+    <t>ASCTEST37</t>
+  </si>
+  <si>
+    <t>ASCTEST38</t>
+  </si>
+  <si>
+    <t>ASCTEST39</t>
+  </si>
+  <si>
+    <t>ASCTEST40</t>
+  </si>
+  <si>
+    <t>ASCTEST41</t>
+  </si>
+  <si>
+    <t>ASCTEST42</t>
+  </si>
+  <si>
+    <t>ASCTEST43</t>
+  </si>
+  <si>
+    <t>ASCTEST44</t>
+  </si>
+  <si>
+    <t>ASCTEST45</t>
+  </si>
+  <si>
+    <t>ASCTEST46</t>
+  </si>
+  <si>
+    <t>ASCTEST47</t>
+  </si>
+  <si>
+    <t>ASCTEST48</t>
+  </si>
+  <si>
+    <t>ASCTEST49</t>
+  </si>
+  <si>
+    <t>ASCTEST50</t>
+  </si>
+  <si>
+    <t>ASCTEST51</t>
+  </si>
+  <si>
+    <t>ASCTEST52</t>
+  </si>
+  <si>
+    <t>ASCTEST53</t>
+  </si>
+  <si>
+    <t>ASCTEST54</t>
+  </si>
+  <si>
+    <t>ASCTEST55</t>
+  </si>
+  <si>
+    <t>ASCTEST56</t>
+  </si>
+  <si>
+    <t>ASCTEST57</t>
+  </si>
+  <si>
+    <t>ASCTEST58</t>
+  </si>
+  <si>
+    <t>ASCTEST59</t>
+  </si>
+  <si>
+    <t>ASCTEST60</t>
+  </si>
+  <si>
+    <t>ASCTEST61</t>
+  </si>
+  <si>
+    <t>ASCTEST62</t>
+  </si>
+  <si>
+    <t>ASCTEST63</t>
+  </si>
+  <si>
+    <t>ASCTEST64</t>
+  </si>
+  <si>
+    <t>ASCTEST65</t>
+  </si>
+  <si>
+    <t>ASCTEST66</t>
+  </si>
+  <si>
+    <t>ASCTEST67</t>
+  </si>
+  <si>
+    <t>ASCTEST68</t>
+  </si>
+  <si>
+    <t>ASCTEST69</t>
+  </si>
+  <si>
+    <t>ASCTEST70</t>
+  </si>
+  <si>
+    <t>ASCTEST71</t>
+  </si>
+  <si>
+    <t>ASCTEST72</t>
+  </si>
+  <si>
+    <t>ASCTEST73</t>
+  </si>
+  <si>
+    <t>ASCTEST74</t>
+  </si>
+  <si>
+    <t>ASCTEST75</t>
+  </si>
+  <si>
+    <t>ASCTEST76</t>
+  </si>
+  <si>
+    <t>ASCTEST77</t>
+  </si>
+  <si>
+    <t>ASCTEST78</t>
+  </si>
+  <si>
+    <t>ASCTEST79</t>
+  </si>
+  <si>
+    <t>ASCTEST80</t>
+  </si>
+  <si>
+    <t>ASCTEST81</t>
+  </si>
+  <si>
+    <t>ASCTEST82</t>
+  </si>
+  <si>
+    <t>ASCTEST83</t>
+  </si>
+  <si>
+    <t>ASCTEST84</t>
+  </si>
+  <si>
+    <t>ASCTEST85</t>
+  </si>
+  <si>
+    <t>ASCTEST86</t>
+  </si>
+  <si>
+    <t>ASCTEST87</t>
+  </si>
+  <si>
+    <t>ASCTEST88</t>
+  </si>
+  <si>
+    <t>ASCTEST89</t>
+  </si>
+  <si>
+    <t>ASCTEST90</t>
+  </si>
+  <si>
+    <t>ASCTEST91</t>
+  </si>
+  <si>
+    <t>ASCTEST92</t>
+  </si>
+  <si>
+    <t>ASCTEST93</t>
+  </si>
+  <si>
+    <t>ASCTEST94</t>
+  </si>
+  <si>
+    <t>ASCTEST95</t>
+  </si>
+  <si>
+    <t>ASCTEST96</t>
+  </si>
+  <si>
+    <t>ASCTEST97</t>
+  </si>
+  <si>
+    <t>ASCTEST98</t>
+  </si>
+  <si>
+    <t>ASCTEST99</t>
+  </si>
+  <si>
+    <t>ASCTEST100</t>
+  </si>
+  <si>
+    <t>ASCTEST101</t>
+  </si>
+  <si>
+    <t>ASCTEST102</t>
+  </si>
+  <si>
+    <t>ASCTEST103</t>
+  </si>
+  <si>
+    <t>ASCTEST104</t>
+  </si>
+  <si>
+    <t>ASCTEST105</t>
+  </si>
+  <si>
+    <t>ASCTEST106</t>
+  </si>
+  <si>
+    <t>ASCTEST107</t>
+  </si>
+  <si>
+    <t>ASCTEST108</t>
+  </si>
+  <si>
+    <t>ASCTEST109</t>
+  </si>
+  <si>
+    <t>ASCTEST110</t>
+  </si>
+  <si>
+    <t>Email Sent</t>
+  </si>
+  <si>
+    <t>Phone number</t>
+  </si>
+  <si>
+    <t>Order nr.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -404,37 +740,590 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E613A84B-28F4-4A13-A0CF-8705EBBCB961}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:F111"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="4" max="4" width="12.265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.46484375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
+        <v>114</v>
+      </c>
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A2" t="s">
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
         <v>5</v>
       </c>
     </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A14" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A15" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A16" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A17" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A18" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A20" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A21" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A22" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A23" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A24" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A25" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A26" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A27" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A28" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A29" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A30" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A31" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A32" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A33" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A34" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A35" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A36" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A37" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A38" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A39" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A40" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A41" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A42" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A43" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A44" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A45" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A46" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A47" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A48" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A49" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A50" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A51" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A52" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A53" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A54" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A55" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A56" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A57" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A58" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A59" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A60" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A61" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A62" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A63" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A64" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A65" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A66" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A67" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A68" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A69" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A70" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A71" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A72" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A73" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A74" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A75" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A76" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A77" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A78" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A79" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A80" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A81" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A82" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A83" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A84" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A85" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A86" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A87" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A88" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A89" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A90" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A91" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A92" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A93" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A94" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A95" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A96" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A97" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A98" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A99" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A100" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A101" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A102" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A103" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A104" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A105" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A106" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A107" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A108" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A109" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A110" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A111" t="s">
+        <v>112</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>